<commit_message>
update colors with fishualize!
</commit_message>
<xml_diff>
--- a/processed/PI_CU_spatial_gfi_summary.xlsx
+++ b/processed/PI_CU_spatial_gfi_summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Vanessa/Desktop/msc_project/processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E210233-33F2-FA45-BF29-2DC28F1487FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D11E4CB-1139-C04E-B408-C5C6373E29BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19460" yWindow="9560" windowWidth="28040" windowHeight="16160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="spatial_gfi_means" sheetId="1" r:id="rId1"/>
@@ -955,7 +955,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="C19" sqref="C19:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>